<commit_message>
Correciones bd agregado campo clase en tematicas.
</commit_message>
<xml_diff>
--- a/db/ExcelTematicas.xlsx
+++ b/db/ExcelTematicas.xlsx
@@ -1,20 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JOEL BR\Documents\CUCEI\Proyecto Modular\CourseRoom\db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java Projects\CourseRoom\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5D9E6B-3D12-4B63-948C-AAD5B732B817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1179,7 +1192,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1739,7 +1752,7 @@
     <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Buena" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
@@ -2039,10 +2052,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H361"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D361"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2080,8 +2095,8 @@
         <v>365</v>
       </c>
       <c r="D2" s="1" t="str">
-        <f>CONCATENATE("INSERT INTO tb_tematicas VALUES (",A2,",",B2,",",C2,");")</f>
-        <v>INSERT INTO tb_tematicas VALUES (1,ABOGACÍA,ESTUDIOS JURIDICOS);</v>
+        <f>CONCATENATE("INSERT INTO `courseroom`.`tb_tematicas` VALUES (",A2,",'",B2,"','",C2,"');")</f>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (1,'ABOGACÍA','ESTUDIOS JURIDICOS');</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2096,8 +2111,8 @@
         <v>369</v>
       </c>
       <c r="D3" s="1" t="str">
-        <f t="shared" ref="D3:D66" si="1">CONCATENATE("INSERT INTO tb_tematicas VALUES (",A3,",",B3,",",C3,");")</f>
-        <v>INSERT INTO tb_tematicas VALUES (2,ACTUARIA,ECONOMIA Y SOCIEDAD);</v>
+        <f t="shared" ref="D3:D66" si="1">CONCATENATE("INSERT INTO `courseroom`.`tb_tematicas` VALUES (",A3,",'",B3,"','",C3,"');")</f>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (2,'ACTUARIA','ECONOMIA Y SOCIEDAD');</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6" t="s">
@@ -2117,7 +2132,7 @@
       </c>
       <c r="D4" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (3,ADMINISTRACIÓN,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (3,'ADMINISTRACIÓN','GESTION EMPRESARIAL');</v>
       </c>
       <c r="F4" s="5">
         <f>ROW(A1)</f>
@@ -2140,7 +2155,7 @@
       </c>
       <c r="D5" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (4,ADMINISTRACIÓN AGRARIA,AGRONOMIA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (4,'ADMINISTRACIÓN AGRARIA','AGRONOMIA');</v>
       </c>
       <c r="F5" s="4">
         <f t="shared" ref="F5:F24" si="2">ROW(A2)</f>
@@ -2163,7 +2178,7 @@
       </c>
       <c r="D6" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (5,ADMINISTRACIÓN AGROPECUARIA,AGRONOMIA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (5,'ADMINISTRACIÓN AGROPECUARIA','AGRONOMIA');</v>
       </c>
       <c r="F6" s="4">
         <f t="shared" si="2"/>
@@ -2186,7 +2201,7 @@
       </c>
       <c r="D7" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (6,ADMINISTRACIÓN DE EMPRESAS,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (6,'ADMINISTRACIÓN DE EMPRESAS','GESTION EMPRESARIAL');</v>
       </c>
       <c r="F7" s="4">
         <f t="shared" si="2"/>
@@ -2209,7 +2224,7 @@
       </c>
       <c r="D8" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (7,ADMINISTRACIÓN DE NEGOCIOS,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (7,'ADMINISTRACIÓN DE NEGOCIOS','GESTION EMPRESARIAL');</v>
       </c>
       <c r="F8" s="4">
         <f t="shared" si="2"/>
@@ -2232,7 +2247,7 @@
       </c>
       <c r="D9" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (8,ADMINISTRACIÓN DE ORGANIZACIONES DE SALUD,DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (8,'ADMINISTRACIÓN DE ORGANIZACIONES DE SALUD','DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD');</v>
       </c>
       <c r="F9" s="4">
         <f t="shared" si="2"/>
@@ -2255,7 +2270,7 @@
       </c>
       <c r="D10" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (9,ADMINISTRACIÓN DE POLÍTICAS PÚBLICAS,ECONOMIA Y SOCIEDAD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (9,'ADMINISTRACIÓN DE POLÍTICAS PÚBLICAS','ECONOMIA Y SOCIEDAD');</v>
       </c>
       <c r="F10" s="4">
         <f t="shared" si="2"/>
@@ -2278,7 +2293,7 @@
       </c>
       <c r="D11" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (10,ADMINISTRACIÓN DE POLÍTICAS PÚBLICAS LOCALES,ECONOMIA Y SOCIEDAD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (10,'ADMINISTRACIÓN DE POLÍTICAS PÚBLICAS LOCALES','ECONOMIA Y SOCIEDAD');</v>
       </c>
       <c r="F11" s="4">
         <f t="shared" si="2"/>
@@ -2301,7 +2316,7 @@
       </c>
       <c r="D12" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (11,ADMINISTRACIÓN DE SISTEMAS,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (11,'ADMINISTRACIÓN DE SISTEMAS','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
       <c r="F12" s="4">
         <f t="shared" si="2"/>
@@ -2325,7 +2340,7 @@
       </c>
       <c r="D13" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (12,ADMINISTRACIÓN EDUCATIVA,CIENCIAS DE LA EDUCACION);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (12,'ADMINISTRACIÓN EDUCATIVA','CIENCIAS DE LA EDUCACION');</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="4">
@@ -2349,7 +2364,7 @@
       </c>
       <c r="D14" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (13,ADMINISTRACIÓN FINANCIERA,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (13,'ADMINISTRACIÓN FINANCIERA','GESTION EMPRESARIAL');</v>
       </c>
       <c r="F14" s="4">
         <f t="shared" si="2"/>
@@ -2372,7 +2387,7 @@
       </c>
       <c r="D15" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (14,ADMINISTRACIÓN GUBERNAMENTAL,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (14,'ADMINISTRACIÓN GUBERNAMENTAL','GESTION EMPRESARIAL');</v>
       </c>
       <c r="F15" s="4">
         <f t="shared" si="2"/>
@@ -2395,7 +2410,7 @@
       </c>
       <c r="D16" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (15,ADMINISTRACIÓN PÚBLICA,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (15,'ADMINISTRACIÓN PÚBLICA','GESTION EMPRESARIAL');</v>
       </c>
       <c r="F16" s="4">
         <f t="shared" si="2"/>
@@ -2418,7 +2433,7 @@
       </c>
       <c r="D17" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (16,ADMINISTRACIÓN URBANA,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (16,'ADMINISTRACIÓN URBANA','GESTION EMPRESARIAL');</v>
       </c>
       <c r="F17" s="4">
         <f t="shared" si="2"/>
@@ -2441,7 +2456,7 @@
       </c>
       <c r="D18" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (17,ADUANAS,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (17,'ADUANAS','GESTION EMPRESARIAL');</v>
       </c>
       <c r="F18" s="4">
         <f t="shared" si="2"/>
@@ -2464,7 +2479,7 @@
       </c>
       <c r="D19" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (18,AGROBIOTECNOLOGÍA,AGRONOMIA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (18,'AGROBIOTECNOLOGÍA','AGRONOMIA');</v>
       </c>
       <c r="F19" s="4">
         <f t="shared" si="2"/>
@@ -2487,7 +2502,7 @@
       </c>
       <c r="D20" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (19,AGRONEGOCIOS,AGRONOMIA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (19,'AGRONEGOCIOS','AGRONOMIA');</v>
       </c>
       <c r="F20" s="4">
         <f t="shared" si="2"/>
@@ -2510,7 +2525,7 @@
       </c>
       <c r="D21" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (20,ALIMENTOS Y BEBIDAS,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (20,'ALIMENTOS Y BEBIDAS','DISCIPLINAS CLINICAS');</v>
       </c>
       <c r="F21" s="4">
         <f t="shared" si="2"/>
@@ -2533,7 +2548,7 @@
       </c>
       <c r="D22" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (21,ANÁLISIS DE SISTEMAS,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (21,'ANÁLISIS DE SISTEMAS','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
       <c r="F22" s="4">
         <f t="shared" si="2"/>
@@ -2556,7 +2571,7 @@
       </c>
       <c r="D23" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (22,ANÁLISIS DE SISTEMAS INFORMÁTICOS,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (22,'ANÁLISIS DE SISTEMAS INFORMÁTICOS','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
       <c r="F23" s="4">
         <f t="shared" si="2"/>
@@ -2579,7 +2594,7 @@
       </c>
       <c r="D24" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (23,ANESTESIOLOGÍA PEDIÁTRICA,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (23,'ANESTESIOLOGÍA PEDIÁTRICA','DISCIPLINAS CLINICAS');</v>
       </c>
       <c r="F24" s="4">
         <f t="shared" si="2"/>
@@ -2602,7 +2617,7 @@
       </c>
       <c r="D25" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (24,ANTROPOLOGÍA,ESTUDIOS HISTORICOS Y HUMANOS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (24,'ANTROPOLOGÍA','ESTUDIOS HISTORICOS Y HUMANOS');</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2618,7 +2633,7 @@
       </c>
       <c r="D26" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (25,ANTROPOLOGÍA FÍSICA,ESTUDIOS HISTORICOS Y HUMANOS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (25,'ANTROPOLOGÍA FÍSICA','ESTUDIOS HISTORICOS Y HUMANOS');</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2634,7 +2649,7 @@
       </c>
       <c r="D27" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (26,ARCHIVONOMÍA,ESTUDIOS DE LA CULTURA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (26,'ARCHIVONOMÍA','ESTUDIOS DE LA CULTURA');</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2650,7 +2665,7 @@
       </c>
       <c r="D28" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (27,ARQUEOLOGÍA,ESTUDIOS HISTORICOS Y HUMANOS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (27,'ARQUEOLOGÍA','ESTUDIOS HISTORICOS Y HUMANOS');</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2666,7 +2681,7 @@
       </c>
       <c r="D29" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (28,ARQUITECTURA,IMAGEN Y SONIDO);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (28,'ARQUITECTURA','IMAGEN Y SONIDO');</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2682,7 +2697,7 @@
       </c>
       <c r="D30" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (29,ARTE,ARTES VISUALES);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (29,'ARTE','ARTES VISUALES');</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2698,7 +2713,7 @@
       </c>
       <c r="D31" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (30,ARTES AUDIOVISUALES,ARTES VISUALES);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (30,'ARTES AUDIOVISUALES','ARTES VISUALES');</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2714,7 +2729,7 @@
       </c>
       <c r="D32" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (31,ARTES ESCÉNICAS PARA LA EXPRESIÓN DANCÍSTICA,ARTES ESCENICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (31,'ARTES ESCÉNICAS PARA LA EXPRESIÓN DANCÍSTICA','ARTES ESCENICAS');</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2730,7 +2745,7 @@
       </c>
       <c r="D33" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (32,ARTES ESCÉNICAS PARA LA EXPRESIÓN TEATRAL,ARTES ESCENICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (32,'ARTES ESCÉNICAS PARA LA EXPRESIÓN TEATRAL','ARTES ESCENICAS');</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2746,7 +2761,7 @@
       </c>
       <c r="D34" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (33,ARTES VISUALES PARA LA EXPRESIÓN FOTOGRÁFICA,ARTES VISUALES);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (33,'ARTES VISUALES PARA LA EXPRESIÓN FOTOGRÁFICA','ARTES VISUALES');</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2762,7 +2777,7 @@
       </c>
       <c r="D35" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (34,ARTES VISUALES PARA LA EXPRESIÓN PLÁSTICA,ARTES VISUALES);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (34,'ARTES VISUALES PARA LA EXPRESIÓN PLÁSTICA','ARTES VISUALES');</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2778,7 +2793,7 @@
       </c>
       <c r="D36" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (35,ASISTENTE DIRECTIVO,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (35,'ASISTENTE DIRECTIVO','GESTION EMPRESARIAL');</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2794,7 +2809,7 @@
       </c>
       <c r="D37" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (36,ASISTENTE EJECUTIVO,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (36,'ASISTENTE EJECUTIVO','GESTION EMPRESARIAL');</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2810,7 +2825,7 @@
       </c>
       <c r="D38" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (37,AUDIOLOGÍA,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (37,'AUDIOLOGÍA','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2826,7 +2841,7 @@
       </c>
       <c r="D39" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (38,BIBLIOTECOLOGÍA,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (38,'BIBLIOTECOLOGÍA','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2842,7 +2857,7 @@
       </c>
       <c r="D40" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (39,BIOINGENIERÍA,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (39,'BIOINGENIERÍA','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2858,7 +2873,7 @@
       </c>
       <c r="D41" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (40,BIOLOGÍA,CIENCIAS BASICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (40,'BIOLOGÍA','CIENCIAS BASICAS');</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2874,7 +2889,7 @@
       </c>
       <c r="D42" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (41,BIOLOGÍA EXPERIMENTAL,BIOLOGIA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (41,'BIOLOGÍA EXPERIMENTAL','BIOLOGIA');</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2890,7 +2905,7 @@
       </c>
       <c r="D43" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (42,BIOLOGÍA MARINA,BIOLOGIA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (42,'BIOLOGÍA MARINA','BIOLOGIA');</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2906,7 +2921,7 @@
       </c>
       <c r="D44" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (43,BIOMÉDICA,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (43,'BIOMÉDICA','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2922,7 +2937,7 @@
       </c>
       <c r="D45" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (44,BIOMEDICINA BÁSICA,CIENCIAS BASICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (44,'BIOMEDICINA BÁSICA','CIENCIAS BASICAS');</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2938,7 +2953,7 @@
       </c>
       <c r="D46" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (45,BIOMEDICINA EXPERIMENTAL,CIENCIAS BASICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (45,'BIOMEDICINA EXPERIMENTAL','CIENCIAS BASICAS');</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2954,7 +2969,7 @@
       </c>
       <c r="D47" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (46,BIOQUÍMICA DIAGNOSTICA,CIENCIAS BASICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (46,'BIOQUÍMICA DIAGNOSTICA','CIENCIAS BASICAS');</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2970,7 +2985,7 @@
       </c>
       <c r="D48" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (47,BIOTECNOLOGÍA,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (47,'BIOTECNOLOGÍA','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2986,7 +3001,7 @@
       </c>
       <c r="D49" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (48,CARDIOLOGÍA PEDIÁTRICA,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (48,'CARDIOLOGÍA PEDIÁTRICA','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3002,7 +3017,7 @@
       </c>
       <c r="D50" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (49,CIENCIA DE DATOS,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (49,'CIENCIA DE DATOS','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3018,7 +3033,7 @@
       </c>
       <c r="D51" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (50,CIENCIA DE EDIFICACIÓN,INGENIERIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (50,'CIENCIA DE EDIFICACIÓN','INGENIERIAS');</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3034,7 +3049,7 @@
       </c>
       <c r="D52" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (51,CIENCIA DE LOS ALIMENTOS,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (51,'CIENCIA DE LOS ALIMENTOS','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3050,7 +3065,7 @@
       </c>
       <c r="D53" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (52,CIENCIA Y TECNOLOGÍA,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (52,'CIENCIA Y TECNOLOGÍA','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3066,7 +3081,7 @@
       </c>
       <c r="D54" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (53,CIENCIAS ADMINISTRATIVAS,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (53,'CIENCIAS ADMINISTRATIVAS','GESTION EMPRESARIAL');</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3082,7 +3097,7 @@
       </c>
       <c r="D55" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (54,CIENCIAS AGRARIAS,AGRONOMIA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (54,'CIENCIAS AGRARIAS','AGRONOMIA');</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3098,7 +3113,7 @@
       </c>
       <c r="D56" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (55,CIENCIAS AGROPECUARIAS,AGRONOMIA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (55,'CIENCIAS AGROPECUARIAS','AGRONOMIA');</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3114,7 +3129,7 @@
       </c>
       <c r="D57" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (56,CIENCIAS APLICADAS,CIENCIAS BASICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (56,'CIENCIAS APLICADAS','CIENCIAS BASICAS');</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3130,7 +3145,7 @@
       </c>
       <c r="D58" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (57,CIENCIAS BIOLÓGICAS,BIOLOGIA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (57,'CIENCIAS BIOLÓGICAS','BIOLOGIA');</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3146,7 +3161,7 @@
       </c>
       <c r="D59" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (58,CIENCIAS BIOMÉDICAS,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (58,'CIENCIAS BIOMÉDICAS','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3162,7 +3177,7 @@
       </c>
       <c r="D60" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (59,CIENCIAS CONTABLES,CONTADURIA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (59,'CIENCIAS CONTABLES','CONTADURIA');</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3178,7 +3193,7 @@
       </c>
       <c r="D61" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (60,CIENCIAS DE AUDITORIA,CONTADURIA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (60,'CIENCIAS DE AUDITORIA','CONTADURIA');</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3194,7 +3209,7 @@
       </c>
       <c r="D62" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (61,CIENCIAS DE LA COMUNICACIÓN,INGENIERIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (61,'CIENCIAS DE LA COMUNICACIÓN','INGENIERIAS');</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3210,7 +3225,7 @@
       </c>
       <c r="D63" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (62,CIENCIAS DE LA EDUCACIÓN,CIENCIAS DE LA EDUCACION);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (62,'CIENCIAS DE LA EDUCACIÓN','CIENCIAS DE LA EDUCACION');</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3226,7 +3241,7 @@
       </c>
       <c r="D64" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (63,CIENCIAS DE LA EMPRESA,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (63,'CIENCIAS DE LA EMPRESA','GESTION EMPRESARIAL');</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3242,7 +3257,7 @@
       </c>
       <c r="D65" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (64,CIENCIAS DE LA INFORMÁTICA,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (64,'CIENCIAS DE LA INFORMÁTICA','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3258,7 +3273,7 @@
       </c>
       <c r="D66" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tb_tematicas VALUES (65,CIENCIAS DE LA PRODUCCIÓN,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (65,'CIENCIAS DE LA PRODUCCIÓN','GESTION EMPRESARIAL');</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3273,8 +3288,8 @@
         <v>380</v>
       </c>
       <c r="D67" s="1" t="str">
-        <f t="shared" ref="D67:D130" si="4">CONCATENATE("INSERT INTO tb_tematicas VALUES (",A67,",",B67,",",C67,");")</f>
-        <v>INSERT INTO tb_tematicas VALUES (66,CIENCIAS DE LA SALUD,DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD);</v>
+        <f t="shared" ref="D67:D130" si="4">CONCATENATE("INSERT INTO `courseroom`.`tb_tematicas` VALUES (",A67,",'",B67,"','",C67,"');")</f>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (66,'CIENCIAS DE LA SALUD','DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD');</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3290,7 +3305,7 @@
       </c>
       <c r="D68" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (67,CIENCIAS DEL ARTE,IMAGEN Y SONIDO);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (67,'CIENCIAS DEL ARTE','IMAGEN Y SONIDO');</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3306,7 +3321,7 @@
       </c>
       <c r="D69" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (68,CIENCIAS DEL DEPORTE,DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (68,'CIENCIAS DEL DEPORTE','DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD');</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3322,7 +3337,7 @@
       </c>
       <c r="D70" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (69,CIENCIAS DIPLOMÁTICAS,ESTUDIOS POLITICOS Y SOCIALES);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (69,'CIENCIAS DIPLOMÁTICAS','ESTUDIOS POLITICOS Y SOCIALES');</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3338,7 +3353,7 @@
       </c>
       <c r="D71" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (70,CIENCIAS ECONÓMICAS,ECONOMIA Y SOCIEDAD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (70,'CIENCIAS ECONÓMICAS','ECONOMIA Y SOCIEDAD');</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3354,7 +3369,7 @@
       </c>
       <c r="D72" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (71,CIENCIAS EMPRESARIALES,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (71,'CIENCIAS EMPRESARIALES','GESTION EMPRESARIAL');</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3370,7 +3385,7 @@
       </c>
       <c r="D73" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (72,CIENCIAS FARMACÉUTICAS,CIENCIAS BASICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (72,'CIENCIAS FARMACÉUTICAS','CIENCIAS BASICAS');</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3386,7 +3401,7 @@
       </c>
       <c r="D74" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (73,CIENCIAS FORESTALES,INGENIERIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (73,'CIENCIAS FORESTALES','INGENIERIAS');</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3402,7 +3417,7 @@
       </c>
       <c r="D75" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (74,CIENCIAS HUMANAS,ESTUDIOS HISTORICOS Y HUMANOS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (74,'CIENCIAS HUMANAS','ESTUDIOS HISTORICOS Y HUMANOS');</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3418,7 +3433,7 @@
       </c>
       <c r="D76" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (75,CIENCIAS INFORMÁTICAS,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (75,'CIENCIAS INFORMÁTICAS','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3434,7 +3449,7 @@
       </c>
       <c r="D77" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (76,CIENCIAS JURÍDICAS,ESTUDIOS JURIDICOS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (76,'CIENCIAS JURÍDICAS','ESTUDIOS JURIDICOS');</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3450,7 +3465,7 @@
       </c>
       <c r="D78" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (77,CIENCIAS MÉDICAS,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (77,'CIENCIAS MÉDICAS','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3466,7 +3481,7 @@
       </c>
       <c r="D79" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (78,CIENCIAS POLÍTICAS,ESTUDIOS POLITICOS Y SOCIALES);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (78,'CIENCIAS POLÍTICAS','ESTUDIOS POLITICOS Y SOCIALES');</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3482,7 +3497,7 @@
       </c>
       <c r="D80" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (79,CIENCIAS QUÍMICAS,CIENCIAS BASICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (79,'CIENCIAS QUÍMICAS','CIENCIAS BASICAS');</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3498,7 +3513,7 @@
       </c>
       <c r="D81" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (80,CIENCIAS QUIMICOBIOLOGICAS,CIENCIAS BASICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (80,'CIENCIAS QUIMICOBIOLOGICAS','CIENCIAS BASICAS');</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3514,7 +3529,7 @@
       </c>
       <c r="D82" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (81,CIENCIAS SOCIALES,ESTUDIOS POLITICOS Y SOCIALES);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (81,'CIENCIAS SOCIALES','ESTUDIOS POLITICOS Y SOCIALES');</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3530,7 +3545,7 @@
       </c>
       <c r="D83" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (82,CIENCIAS TECNOLOGÍCAS,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (82,'CIENCIAS TECNOLOGÍCAS','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3546,7 +3561,7 @@
       </c>
       <c r="D84" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (83,CIENCIAS VETERINARIAS,CIENCIAS VETERINARIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (83,'CIENCIAS VETERINARIAS','CIENCIAS VETERINARIAS');</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3562,7 +3577,7 @@
       </c>
       <c r="D85" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (84,CIENCIAS Y ARTE,IMAGEN Y SONIDO);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (84,'CIENCIAS Y ARTE','IMAGEN Y SONIDO');</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3578,7 +3593,7 @@
       </c>
       <c r="D86" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (85,CINEMATOGRAFÍA,ARTES VISUALES);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (85,'CINEMATOGRAFÍA','ARTES VISUALES');</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3594,7 +3609,7 @@
       </c>
       <c r="D87" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (86,CIRUGÍA PLÁSTICA ESTÉTICA,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (86,'CIRUGÍA PLÁSTICA ESTÉTICA','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3610,7 +3625,7 @@
       </c>
       <c r="D88" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (87,CIRUGÍA PLÁSTICA RECONSTRUCTIVA,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (87,'CIRUGÍA PLÁSTICA RECONSTRUCTIVA','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3626,7 +3641,7 @@
       </c>
       <c r="D89" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (88,CIRUJANO DENTISTA,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (88,'CIRUJANO DENTISTA','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3642,7 +3657,7 @@
       </c>
       <c r="D90" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (89,COMERCIALIZACIÓN,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (89,'COMERCIALIZACIÓN','GESTION EMPRESARIAL');</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3658,7 +3673,7 @@
       </c>
       <c r="D91" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (90,COMERCIO EXTERIOR,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (90,'COMERCIO EXTERIOR','GESTION EMPRESARIAL');</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3674,7 +3689,7 @@
       </c>
       <c r="D92" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (91,COMERCIO INTERNACIONAL,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (91,'COMERCIO INTERNACIONAL','GESTION EMPRESARIAL');</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3690,7 +3705,7 @@
       </c>
       <c r="D93" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (92,COMPOSICIÓN,IMAGEN Y SONIDO);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (92,'COMPOSICIÓN','IMAGEN Y SONIDO');</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3706,7 +3721,7 @@
       </c>
       <c r="D94" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (93,COMPUTACIÓN,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (93,'COMPUTACIÓN','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3722,7 +3737,7 @@
       </c>
       <c r="D95" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (94,COMUNICACIÓN AUDIOVISUAL,ESTUDIOS DE LA CULTURA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (94,'COMUNICACIÓN AUDIOVISUAL','ESTUDIOS DE LA CULTURA');</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3738,7 +3753,7 @@
       </c>
       <c r="D96" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (95,COMUNICACIÓN HUMANA,ESTUDIOS DE LA CULTURA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (95,'COMUNICACIÓN HUMANA','ESTUDIOS DE LA CULTURA');</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3754,7 +3769,7 @@
       </c>
       <c r="D97" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (96,COMUNICACIÓN PÚBLICA,ESTUDIOS DE LA CULTURA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (96,'COMUNICACIÓN PÚBLICA','ESTUDIOS DE LA CULTURA');</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3770,7 +3785,7 @@
       </c>
       <c r="D98" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (97,COMUNICACIÓN SOCIAL,ESTUDIOS DE LA CULTURA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (97,'COMUNICACIÓN SOCIAL','ESTUDIOS DE LA CULTURA');</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3786,7 +3801,7 @@
       </c>
       <c r="D99" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (98,COMUNICACIÓN VISUAL,ESTUDIOS DE LA CULTURA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (98,'COMUNICACIÓN VISUAL','ESTUDIOS DE LA CULTURA');</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3802,7 +3817,7 @@
       </c>
       <c r="D100" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (99,CONSTRUCCIÓN,INGENIERIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (99,'CONSTRUCCIÓN','INGENIERIAS');</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3818,7 +3833,7 @@
       </c>
       <c r="D101" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (100,CONTABILIDAD,CONTADURIA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (100,'CONTABILIDAD','CONTADURIA');</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3834,7 +3849,7 @@
       </c>
       <c r="D102" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (101,CONTABILIDAD FINANCIERA,CONTADURIA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (101,'CONTABILIDAD FINANCIERA','CONTADURIA');</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3850,7 +3865,7 @@
       </c>
       <c r="D103" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (102,CONTABILIDAD FISCAL,CONTADURIA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (102,'CONTABILIDAD FISCAL','CONTADURIA');</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3866,7 +3881,7 @@
       </c>
       <c r="D104" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (103,CONTABILIDAD PÚBLICA,CONTADURIA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (103,'CONTABILIDAD PÚBLICA','CONTADURIA');</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3882,7 +3897,7 @@
       </c>
       <c r="D105" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (104,CONTADOR PRIVADO,CONTADURIA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (104,'CONTADOR PRIVADO','CONTADURIA');</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3898,7 +3913,7 @@
       </c>
       <c r="D106" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (105,CONTADOR PÚBLICO,CONTADURIA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (105,'CONTADOR PÚBLICO','CONTADURIA');</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3914,7 +3929,7 @@
       </c>
       <c r="D107" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (106,CONTADOR PÚBLICO NACIONAL,CONTADURIA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (106,'CONTADOR PÚBLICO NACIONAL','CONTADURIA');</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3930,7 +3945,7 @@
       </c>
       <c r="D108" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (107,CONTADURÍA,CONTADURIA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (107,'CONTADURÍA','CONTADURIA');</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3946,7 +3961,7 @@
       </c>
       <c r="D109" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (108,CONTADURÍA PRIVADA,CONTADURIA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (108,'CONTADURÍA PRIVADA','CONTADURIA');</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3962,7 +3977,7 @@
       </c>
       <c r="D110" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (109,CONTADURÍA PÚBLICA,CONTADURIA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (109,'CONTADURÍA PÚBLICA','CONTADURIA');</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3978,7 +3993,7 @@
       </c>
       <c r="D111" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (110,CRIMINALÍSTICA,ESTUDIOS POLITICOS Y SOCIALES);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (110,'CRIMINALÍSTICA','ESTUDIOS POLITICOS Y SOCIALES');</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3994,7 +4009,7 @@
       </c>
       <c r="D112" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (111,CRIMINOLOGÍA,ESTUDIOS POLITICOS Y SOCIALES);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (111,'CRIMINOLOGÍA','ESTUDIOS POLITICOS Y SOCIALES');</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4010,7 +4025,7 @@
       </c>
       <c r="D113" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (112,CULTURA FÍSICA Y DEPORTES,DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (112,'CULTURA FÍSICA Y DEPORTES','DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD');</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4026,7 +4041,7 @@
       </c>
       <c r="D114" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (113,DERECHO,ESTUDIOS JURIDICOS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (113,'DERECHO','ESTUDIOS JURIDICOS');</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4042,7 +4057,7 @@
       </c>
       <c r="D115" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (114,DERECHO ADMINISTRATIVO,ECONOMIA Y SOCIEDAD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (114,'DERECHO ADMINISTRATIVO','ECONOMIA Y SOCIEDAD');</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4058,7 +4073,7 @@
       </c>
       <c r="D116" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (115,DESARROLLO DEL PRODUCTO,INGENIERIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (115,'DESARROLLO DEL PRODUCTO','INGENIERIAS');</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4074,7 +4089,7 @@
       </c>
       <c r="D117" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (116,DESARROLLO EDUCATIVO,CIENCIAS DE LA EDUCACION);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (116,'DESARROLLO EDUCATIVO','CIENCIAS DE LA EDUCACION');</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4090,7 +4105,7 @@
       </c>
       <c r="D118" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (117,DESARROLLO HUMANO,DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (117,'DESARROLLO HUMANO','DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD');</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4106,7 +4121,7 @@
       </c>
       <c r="D119" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (118,DESARROLLO RURAL,AGRONOMIA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (118,'DESARROLLO RURAL','AGRONOMIA');</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4122,7 +4137,7 @@
       </c>
       <c r="D120" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (119,DIDÁCTICA DEL FRANCÉS COMO LENGUA EXTRANJERA,ESTUDIOS HISTORICOS Y HUMANOS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (119,'DIDÁCTICA DEL FRANCÉS COMO LENGUA EXTRANJERA','ESTUDIOS HISTORICOS Y HUMANOS');</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4138,7 +4153,7 @@
       </c>
       <c r="D121" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (120,DIETÉTICA,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (120,'DIETÉTICA','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4154,7 +4169,7 @@
       </c>
       <c r="D122" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (121,DIRECCIÓN DE PROYECTOS,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (121,'DIRECCIÓN DE PROYECTOS','GESTION EMPRESARIAL');</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4170,7 +4185,7 @@
       </c>
       <c r="D123" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (122,DISEÑO,IMAGEN Y SONIDO);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (122,'DISEÑO','IMAGEN Y SONIDO');</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4186,7 +4201,7 @@
       </c>
       <c r="D124" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (123,DISEÑO ARQUITECTÓNICO,IMAGEN Y SONIDO);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (123,'DISEÑO ARQUITECTÓNICO','IMAGEN Y SONIDO');</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4202,7 +4217,7 @@
       </c>
       <c r="D125" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (124,DISEÑO DE ARTESANÍAS,IMAGEN Y SONIDO);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (124,'DISEÑO DE ARTESANÍAS','IMAGEN Y SONIDO');</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4218,7 +4233,7 @@
       </c>
       <c r="D126" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (125,DISEÑO DE INTERIORES Y AMBIENTACIÓN,IMAGEN Y SONIDO);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (125,'DISEÑO DE INTERIORES Y AMBIENTACIÓN','IMAGEN Y SONIDO');</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4234,7 +4249,7 @@
       </c>
       <c r="D127" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (126,DISEÑO DE MODAS,IMAGEN Y SONIDO);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (126,'DISEÑO DE MODAS','IMAGEN Y SONIDO');</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4250,7 +4265,7 @@
       </c>
       <c r="D128" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (127,DISEÑO GRÁFICO,IMAGEN Y SONIDO);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (127,'DISEÑO GRÁFICO','IMAGEN Y SONIDO');</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4266,7 +4281,7 @@
       </c>
       <c r="D129" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (128,DISEÑO INDUSTRIAL,IMAGEN Y SONIDO);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (128,'DISEÑO INDUSTRIAL','IMAGEN Y SONIDO');</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4282,7 +4297,7 @@
       </c>
       <c r="D130" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>INSERT INTO tb_tematicas VALUES (129,DISEÑO PARA LA COMUNICACIÓN GRÁFICA,IMAGEN Y SONIDO);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (129,'DISEÑO PARA LA COMUNICACIÓN GRÁFICA','IMAGEN Y SONIDO');</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4297,8 +4312,8 @@
         <v>364</v>
       </c>
       <c r="D131" s="1" t="str">
-        <f t="shared" ref="D131:D194" si="6">CONCATENATE("INSERT INTO tb_tematicas VALUES (",A131,",",B131,",",C131,");")</f>
-        <v>INSERT INTO tb_tematicas VALUES (130,DOCENCIA DEL INGLÉS COMO LENGUA EXTRANJERA,ESTUDIOS HISTORICOS Y HUMANOS);</v>
+        <f t="shared" ref="D131:D194" si="6">CONCATENATE("INSERT INTO `courseroom`.`tb_tematicas` VALUES (",A131,",'",B131,"','",C131,"');")</f>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (130,'DOCENCIA DEL INGLÉS COMO LENGUA EXTRANJERA','ESTUDIOS HISTORICOS Y HUMANOS');</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4314,7 +4329,7 @@
       </c>
       <c r="D132" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (131,ECONOMÍA,ECONOMIA Y SOCIEDAD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (131,'ECONOMÍA','ECONOMIA Y SOCIEDAD');</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4330,7 +4345,7 @@
       </c>
       <c r="D133" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (132,EDUCACIÓN (ABIERTA Y A DISTANCIA),CIENCIAS DE LA EDUCACION);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (132,'EDUCACIÓN (ABIERTA Y A DISTANCIA)','CIENCIAS DE LA EDUCACION');</v>
       </c>
     </row>
     <row r="134" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4346,7 +4361,7 @@
       </c>
       <c r="D134" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (133,EDUCACIÓN ESPECIAL,DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (133,'EDUCACIÓN ESPECIAL','DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD');</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4362,7 +4377,7 @@
       </c>
       <c r="D135" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (134,EDUCACIÓN ESPECIAL DE AUDICIÓN,DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (134,'EDUCACIÓN ESPECIAL DE AUDICIÓN','DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD');</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4378,7 +4393,7 @@
       </c>
       <c r="D136" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (135,EDUCACIÓN ESPECIAL DE LENGUAJE,DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (135,'EDUCACIÓN ESPECIAL DE LENGUAJE','DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD');</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4394,7 +4409,7 @@
       </c>
       <c r="D137" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (136,EDUCACIÓN PARA LA SALUD,DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (136,'EDUCACIÓN PARA LA SALUD','DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD');</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4410,7 +4425,7 @@
       </c>
       <c r="D138" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (137,EDUCACIÓN PREESCOLAR,CIENCIAS DE LA EDUCACION);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (137,'EDUCACIÓN PREESCOLAR','CIENCIAS DE LA EDUCACION');</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4426,7 +4441,7 @@
       </c>
       <c r="D139" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (138,EJECUTIVO BILINGÜE,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (138,'EJECUTIVO BILINGÜE','GESTION EMPRESARIAL');</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4442,7 +4457,7 @@
       </c>
       <c r="D140" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (139,ELECTRICIDAD,INGENIERIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (139,'ELECTRICIDAD','INGENIERIAS');</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4458,7 +4473,7 @@
       </c>
       <c r="D141" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (140,ELECTRICISTA,INGENIERIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (140,'ELECTRICISTA','INGENIERIAS');</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4474,7 +4489,7 @@
       </c>
       <c r="D142" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (141,ELECTRÓNICA,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (141,'ELECTRÓNICA','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4490,7 +4505,7 @@
       </c>
       <c r="D143" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (142,ENFERMERA QUIRÚRGICA,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (142,'ENFERMERA QUIRÚRGICA','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="144" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4506,7 +4521,7 @@
       </c>
       <c r="D144" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (143,ENFERMERÍA,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (143,'ENFERMERÍA','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4522,7 +4537,7 @@
       </c>
       <c r="D145" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (144,ENFERMERÍA DEL NEONATO,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (144,'ENFERMERÍA DEL NEONATO','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4538,7 +4553,7 @@
       </c>
       <c r="D146" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (145,ENFERMERÍA GENERAL,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (145,'ENFERMERÍA GENERAL','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4554,7 +4569,7 @@
       </c>
       <c r="D147" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (146,ENFERMERÍA INFANTIL,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (146,'ENFERMERÍA INFANTIL','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4570,7 +4585,7 @@
       </c>
       <c r="D148" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (147,ENFERMERÍA PEDIÁTRICA,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (147,'ENFERMERÍA PEDIÁTRICA','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4586,7 +4601,7 @@
       </c>
       <c r="D149" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (148,ENFERMERÍA PERINATAL,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (148,'ENFERMERÍA PERINATAL','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4602,7 +4617,7 @@
       </c>
       <c r="D150" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (149,ESPECIALISTA EN ORTODONCIA,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (149,'ESPECIALISTA EN ORTODONCIA','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="151" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4618,7 +4633,7 @@
       </c>
       <c r="D151" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (150,ESTADÍSTICA,CIENCIAS BASICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (150,'ESTADÍSTICA','CIENCIAS BASICAS');</v>
       </c>
     </row>
     <row r="152" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4634,7 +4649,7 @@
       </c>
       <c r="D152" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (151,ESTUDIOS ÁRABES,ESTUDIOS DE ESTADO Y SOCIEDAD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (151,'ESTUDIOS ÁRABES','ESTUDIOS DE ESTADO Y SOCIEDAD');</v>
       </c>
     </row>
     <row r="153" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4650,7 +4665,7 @@
       </c>
       <c r="D153" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (152,ESTUDIOS ASIA ORIENTAL,ESTUDIOS DE ESTADO Y SOCIEDAD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (152,'ESTUDIOS ASIA ORIENTAL','ESTUDIOS DE ESTADO Y SOCIEDAD');</v>
       </c>
     </row>
     <row r="154" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4666,7 +4681,7 @@
       </c>
       <c r="D154" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (153,ESTUDIOS DE LA INFORMACIÓN,ESTUDIOS DE ESTADO Y SOCIEDAD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (153,'ESTUDIOS DE LA INFORMACIÓN','ESTUDIOS DE ESTADO Y SOCIEDAD');</v>
       </c>
     </row>
     <row r="155" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4682,7 +4697,7 @@
       </c>
       <c r="D155" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (154,ESTUDIOS FRANCESES,ESTUDIOS DE ESTADO Y SOCIEDAD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (154,'ESTUDIOS FRANCESES','ESTUDIOS DE ESTADO Y SOCIEDAD');</v>
       </c>
     </row>
     <row r="156" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4698,7 +4713,7 @@
       </c>
       <c r="D156" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (155,ESTUDIOS INGLESES,ESTUDIOS DE ESTADO Y SOCIEDAD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (155,'ESTUDIOS INGLESES','ESTUDIOS DE ESTADO Y SOCIEDAD');</v>
       </c>
     </row>
     <row r="157" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4714,7 +4729,7 @@
       </c>
       <c r="D157" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (156,ESTUDIOS ISLÁMICOS,ESTUDIOS DE ESTADO Y SOCIEDAD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (156,'ESTUDIOS ISLÁMICOS','ESTUDIOS DE ESTADO Y SOCIEDAD');</v>
       </c>
     </row>
     <row r="158" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4730,7 +4745,7 @@
       </c>
       <c r="D158" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (157,ESTUDIOS LIBERALES,ESTUDIOS DE ESTADO Y SOCIEDAD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (157,'ESTUDIOS LIBERALES','ESTUDIOS DE ESTADO Y SOCIEDAD');</v>
       </c>
     </row>
     <row r="159" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4746,7 +4761,7 @@
       </c>
       <c r="D159" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (158,ESTUDIOS POLÍTICOS Y GOBIERNO,ESTUDIOS POLITICOS Y SOCIALES);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (158,'ESTUDIOS POLÍTICOS Y GOBIERNO','ESTUDIOS POLITICOS Y SOCIALES');</v>
       </c>
     </row>
     <row r="160" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4762,7 +4777,7 @@
       </c>
       <c r="D160" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (159,FARMACIA,CIENCIAS BASICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (159,'FARMACIA','CIENCIAS BASICAS');</v>
       </c>
     </row>
     <row r="161" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4778,7 +4793,7 @@
       </c>
       <c r="D161" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (160,FILOLOGÍA CLÁSICA,ESTUDIOS HISTORICOS Y HUMANOS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (160,'FILOLOGÍA CLÁSICA','ESTUDIOS HISTORICOS Y HUMANOS');</v>
       </c>
     </row>
     <row r="162" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4794,7 +4809,7 @@
       </c>
       <c r="D162" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (161,FILOLOGÍA HISPÁNICA,ESTUDIOS HISTORICOS Y HUMANOS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (161,'FILOLOGÍA HISPÁNICA','ESTUDIOS HISTORICOS Y HUMANOS');</v>
       </c>
     </row>
     <row r="163" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4810,7 +4825,7 @@
       </c>
       <c r="D163" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (162,FILOSOFÍA,ESTUDIOS HISTORICOS Y HUMANOS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (162,'FILOSOFÍA','ESTUDIOS HISTORICOS Y HUMANOS');</v>
       </c>
     </row>
     <row r="164" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4826,7 +4841,7 @@
       </c>
       <c r="D164" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (163,FISIATRÍA,DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (163,'FISIATRÍA','DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD');</v>
       </c>
     </row>
     <row r="165" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4842,7 +4857,7 @@
       </c>
       <c r="D165" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (164,FÍSICA,CIENCIAS BASICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (164,'FÍSICA','CIENCIAS BASICAS');</v>
       </c>
     </row>
     <row r="166" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4858,7 +4873,7 @@
       </c>
       <c r="D166" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (165,FISIOTERAPIA,DISCIPLINAS BASICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (165,'FISIOTERAPIA','DISCIPLINAS BASICAS');</v>
       </c>
     </row>
     <row r="167" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4874,7 +4889,7 @@
       </c>
       <c r="D167" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (166,FONIATRÍA,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (166,'FONIATRÍA','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="168" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4890,7 +4905,7 @@
       </c>
       <c r="D168" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (167,FOTOGRÁFIA,ARTES VISUALES);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (167,'FOTOGRÁFIA','ARTES VISUALES');</v>
       </c>
     </row>
     <row r="169" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4906,7 +4921,7 @@
       </c>
       <c r="D169" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (168,GASTRONOMÍA,CIENCIAS BASICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (168,'GASTRONOMÍA','CIENCIAS BASICAS');</v>
       </c>
     </row>
     <row r="170" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4922,7 +4937,7 @@
       </c>
       <c r="D170" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (169,GENÉTICA PERINATAL,DISCIPLINAS BASICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (169,'GENÉTICA PERINATAL','DISCIPLINAS BASICAS');</v>
       </c>
     </row>
     <row r="171" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4938,7 +4953,7 @@
       </c>
       <c r="D171" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (170,GEOGRAFÍA,ESTUDIOS HISTORICOS Y HUMANOS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (170,'GEOGRAFÍA','ESTUDIOS HISTORICOS Y HUMANOS');</v>
       </c>
     </row>
     <row r="172" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4954,7 +4969,7 @@
       </c>
       <c r="D172" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (171,GERONTOLOGÍA,DISCIPLINAS BASICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (171,'GERONTOLOGÍA','DISCIPLINAS BASICAS');</v>
       </c>
     </row>
     <row r="173" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4970,7 +4985,7 @@
       </c>
       <c r="D173" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (172,GESTIÓN DE HOTELERÍA,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (172,'GESTIÓN DE HOTELERÍA','GESTION EMPRESARIAL');</v>
       </c>
     </row>
     <row r="174" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4986,7 +5001,7 @@
       </c>
       <c r="D174" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (173,GESTIÓN DE TURISMO,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (173,'GESTIÓN DE TURISMO','GESTION EMPRESARIAL');</v>
       </c>
     </row>
     <row r="175" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5002,7 +5017,7 @@
       </c>
       <c r="D175" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (174,GESTIÓN DEL TERRITORIO,ESTUDIOS HISTORICOS Y HUMANOS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (174,'GESTIÓN DEL TERRITORIO','ESTUDIOS HISTORICOS Y HUMANOS');</v>
       </c>
     </row>
     <row r="176" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5018,7 +5033,7 @@
       </c>
       <c r="D176" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (175,GESTIÓN DIRECTIVA EN SALUD,DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (175,'GESTIÓN DIRECTIVA EN SALUD','DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD');</v>
       </c>
     </row>
     <row r="177" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5034,7 +5049,7 @@
       </c>
       <c r="D177" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (176,GESTIÓN Y ECONOMÍA AMBIENTAL,ECONOMIA Y SOCIEDAD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (176,'GESTIÓN Y ECONOMÍA AMBIENTAL','ECONOMIA Y SOCIEDAD');</v>
       </c>
     </row>
     <row r="178" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5050,7 +5065,7 @@
       </c>
       <c r="D178" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (177,HEMATOLOGÍA PEDIÁTRICA,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (177,'HEMATOLOGÍA PEDIÁTRICA','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="179" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5066,7 +5081,7 @@
       </c>
       <c r="D179" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (178,HISTORIA,ESTUDIOS HISTORICOS Y HUMANOS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (178,'HISTORIA','ESTUDIOS HISTORICOS Y HUMANOS');</v>
       </c>
     </row>
     <row r="180" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5082,7 +5097,7 @@
       </c>
       <c r="D180" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (179,HISTORIA DEL ARTE,ESTUDIOS HISTORICOS Y HUMANOS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (179,'HISTORIA DEL ARTE','ESTUDIOS HISTORICOS Y HUMANOS');</v>
       </c>
     </row>
     <row r="181" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5098,7 +5113,7 @@
       </c>
       <c r="D181" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (180,HOTELERÍA,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (180,'HOTELERÍA','GESTION EMPRESARIAL');</v>
       </c>
     </row>
     <row r="182" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5114,7 +5129,7 @@
       </c>
       <c r="D182" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (181,HUMANIDADES,ESTUDIOS HISTORICOS Y HUMANOS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (181,'HUMANIDADES','ESTUDIOS HISTORICOS Y HUMANOS');</v>
       </c>
     </row>
     <row r="183" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5130,7 +5145,7 @@
       </c>
       <c r="D183" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (182,INDUSTRIA,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (182,'INDUSTRIA','GESTION EMPRESARIAL');</v>
       </c>
     </row>
     <row r="184" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5146,7 +5161,7 @@
       </c>
       <c r="D184" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (183,INFORMÁTICA,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (183,'INFORMÁTICA','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="185" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5162,7 +5177,7 @@
       </c>
       <c r="D185" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (184,INFORMÁTICA ADMINISTRATIVA,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (184,'INFORMÁTICA ADMINISTRATIVA','GESTION EMPRESARIAL');</v>
       </c>
     </row>
     <row r="186" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5178,7 +5193,7 @@
       </c>
       <c r="D186" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (185,INFORMÁTICA EMPRESARIAL,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (185,'INFORMÁTICA EMPRESARIAL','GESTION EMPRESARIAL');</v>
       </c>
     </row>
     <row r="187" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5194,7 +5209,7 @@
       </c>
       <c r="D187" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (186,INFORMÁTICA FINANCIERA,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (186,'INFORMÁTICA FINANCIERA','GESTION EMPRESARIAL');</v>
       </c>
     </row>
     <row r="188" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5210,7 +5225,7 @@
       </c>
       <c r="D188" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (187,INGENIERÍA AEROESPACIAL,INGENIERIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (187,'INGENIERÍA AEROESPACIAL','INGENIERIAS');</v>
       </c>
     </row>
     <row r="189" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5226,7 +5241,7 @@
       </c>
       <c r="D189" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (188,INGENIERÍA AGRÍCOLA,AGRONOMIA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (188,'INGENIERÍA AGRÍCOLA','AGRONOMIA');</v>
       </c>
     </row>
     <row r="190" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5242,7 +5257,7 @@
       </c>
       <c r="D190" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (189,INGENIERÍA AGROINDUSTRIAL,AGRONOMIA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (189,'INGENIERÍA AGROINDUSTRIAL','AGRONOMIA');</v>
       </c>
     </row>
     <row r="191" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5258,7 +5273,7 @@
       </c>
       <c r="D191" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (190,INGENIERÍA AGRONÓMICA,AGRONOMIA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (190,'INGENIERÍA AGRONÓMICA','AGRONOMIA');</v>
       </c>
     </row>
     <row r="192" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5274,7 +5289,7 @@
       </c>
       <c r="D192" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (191,INGENIERÍA AGROPECUARIA,AGRONOMIA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (191,'INGENIERÍA AGROPECUARIA','AGRONOMIA');</v>
       </c>
     </row>
     <row r="193" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5290,7 +5305,7 @@
       </c>
       <c r="D193" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (192,INGENIERÍA AMBIENTAL,INGENIERIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (192,'INGENIERÍA AMBIENTAL','INGENIERIAS');</v>
       </c>
     </row>
     <row r="194" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5306,7 +5321,7 @@
       </c>
       <c r="D194" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO tb_tematicas VALUES (193,INGENIERÍA BIOMÉDICA,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (193,'INGENIERÍA BIOMÉDICA','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="195" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5321,8 +5336,8 @@
         <v>362</v>
       </c>
       <c r="D195" s="1" t="str">
-        <f t="shared" ref="D195:D258" si="8">CONCATENATE("INSERT INTO tb_tematicas VALUES (",A195,",",B195,",",C195,");")</f>
-        <v>INSERT INTO tb_tematicas VALUES (194,INGENIERÍA BIOQUÍMICA,CIENCIAS BASICAS);</v>
+        <f t="shared" ref="D195:D258" si="8">CONCATENATE("INSERT INTO `courseroom`.`tb_tematicas` VALUES (",A195,",'",B195,"','",C195,"');")</f>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (194,'INGENIERÍA BIOQUÍMICA','CIENCIAS BASICAS');</v>
       </c>
     </row>
     <row r="196" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5338,7 +5353,7 @@
       </c>
       <c r="D196" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (195,INGENIERÍA CIVIL,INGENIERIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (195,'INGENIERÍA CIVIL','INGENIERIAS');</v>
       </c>
     </row>
     <row r="197" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5354,7 +5369,7 @@
       </c>
       <c r="D197" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (196,INGENIERÍA COMERCIAL,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (196,'INGENIERÍA COMERCIAL','GESTION EMPRESARIAL');</v>
       </c>
     </row>
     <row r="198" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5370,7 +5385,7 @@
       </c>
       <c r="D198" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (197,INGENIERÍA DE ALIMENTOS,INGENIERIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (197,'INGENIERÍA DE ALIMENTOS','INGENIERIAS');</v>
       </c>
     </row>
     <row r="199" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5386,7 +5401,7 @@
       </c>
       <c r="D199" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (198,INGENIERÍA DE LA ENERGÍA,INGENIERIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (198,'INGENIERÍA DE LA ENERGÍA','INGENIERIAS');</v>
       </c>
     </row>
     <row r="200" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5402,7 +5417,7 @@
       </c>
       <c r="D200" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (199,INGENIERÍA DE LA SALUD,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (199,'INGENIERÍA DE LA SALUD','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="201" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5418,7 +5433,7 @@
       </c>
       <c r="D201" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (200,INGENIERÍA DE LAS TECNOLOGÍAS DE TELECOMUNICACIÓN,INGENIERIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (200,'INGENIERÍA DE LAS TECNOLOGÍAS DE TELECOMUNICACIÓN','INGENIERIAS');</v>
       </c>
     </row>
     <row r="202" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5434,7 +5449,7 @@
       </c>
       <c r="D202" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (201,INGENIERÍA DE MATERIALES,INGENIERIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (201,'INGENIERÍA DE MATERIALES','INGENIERIAS');</v>
       </c>
     </row>
     <row r="203" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5450,7 +5465,7 @@
       </c>
       <c r="D203" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (202,INGENIERÍA DE PROCESOS Y COMERCIO INTERNACIONAL,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (202,'INGENIERÍA DE PROCESOS Y COMERCIO INTERNACIONAL','GESTION EMPRESARIAL');</v>
       </c>
     </row>
     <row r="204" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5466,7 +5481,7 @@
       </c>
       <c r="D204" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (203,INGENIERÍA DEL SOFTWARE,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (203,'INGENIERÍA DEL SOFTWARE','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="205" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5482,7 +5497,7 @@
       </c>
       <c r="D205" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (204,INGENIERÍA ELÉCTRICA,INGENIERIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (204,'INGENIERÍA ELÉCTRICA','INGENIERIAS');</v>
       </c>
     </row>
     <row r="206" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5498,7 +5513,7 @@
       </c>
       <c r="D206" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (205,INGENIERÍA ELECTROMECÁNICA,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (205,'INGENIERÍA ELECTROMECÁNICA','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="207" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5514,7 +5529,7 @@
       </c>
       <c r="D207" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (206,INGENIERÍA ELECTRÓNICA,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (206,'INGENIERÍA ELECTRÓNICA','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="208" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5530,7 +5545,7 @@
       </c>
       <c r="D208" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (207,INGENIERÍA ELECTRÓNICA INDUSTRIAL,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (207,'INGENIERÍA ELECTRÓNICA INDUSTRIAL','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="209" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5546,7 +5561,7 @@
       </c>
       <c r="D209" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (208,INGENIERÍA EMPRESARIAL,INGENIERIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (208,'INGENIERÍA EMPRESARIAL','INGENIERIAS');</v>
       </c>
     </row>
     <row r="210" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5562,7 +5577,7 @@
       </c>
       <c r="D210" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (209,INGENIERÍA EN ADMINISTRACIÓN INDUSTRIAL,INGENIERIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (209,'INGENIERÍA EN ADMINISTRACIÓN INDUSTRIAL','INGENIERIAS');</v>
       </c>
     </row>
     <row r="211" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5578,7 +5593,7 @@
       </c>
       <c r="D211" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (210,INGENIERÍA EN AGROINDUSTRIA,AGRONOMIA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (210,'INGENIERÍA EN AGROINDUSTRIA','AGRONOMIA');</v>
       </c>
     </row>
     <row r="212" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5594,7 +5609,7 @@
       </c>
       <c r="D212" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (211,INGENIERÍA EN ALIMENTOS Y BIOTECNOLOGÍA,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (211,'INGENIERÍA EN ALIMENTOS Y BIOTECNOLOGÍA','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="213" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5610,7 +5625,7 @@
       </c>
       <c r="D213" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (212,INGENIERÍA EN BIOTECNOLOGÍA,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (212,'INGENIERÍA EN BIOTECNOLOGÍA','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="214" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5626,7 +5641,7 @@
       </c>
       <c r="D214" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (213,INGENIERÍA EN CIENCIAS COMPUTACIONALES,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (213,'INGENIERÍA EN CIENCIAS COMPUTACIONALES','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="215" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5642,7 +5657,7 @@
       </c>
       <c r="D215" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (214,INGENIERÍA EN COMPUTACIÓN,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (214,'INGENIERÍA EN COMPUTACIÓN','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="216" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5658,7 +5673,7 @@
       </c>
       <c r="D216" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (215,INGENIERÍA EN COMUNICACIONES,INGENIERIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (215,'INGENIERÍA EN COMUNICACIONES','INGENIERIAS');</v>
       </c>
     </row>
     <row r="217" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5674,7 +5689,7 @@
       </c>
       <c r="D217" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (216,INGENIERÍA EN COMUNICACIONES Y ELECTRÓNICA,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (216,'INGENIERÍA EN COMUNICACIONES Y ELECTRÓNICA','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="218" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5690,7 +5705,7 @@
       </c>
       <c r="D218" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (217,INGENIERÍA EN ELECTRICIDAD,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (217,'INGENIERÍA EN ELECTRICIDAD','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="219" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5706,7 +5721,7 @@
       </c>
       <c r="D219" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (218,INGENIERÍA EN ELECTRÓNICA,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (218,'INGENIERÍA EN ELECTRÓNICA','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="220" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5722,7 +5737,7 @@
       </c>
       <c r="D220" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (219,INGENIERÍA EN ELECTRÓNICA Y COMPUTACIÓN,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (219,'INGENIERÍA EN ELECTRÓNICA Y COMPUTACIÓN','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="221" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5738,7 +5753,7 @@
       </c>
       <c r="D221" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (220,INGENIERIA EN GESTIÓN EMPRESARIAL,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (220,'INGENIERIA EN GESTIÓN EMPRESARIAL','GESTION EMPRESARIAL');</v>
       </c>
     </row>
     <row r="222" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5754,7 +5769,7 @@
       </c>
       <c r="D222" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (221,INGENIERÍA EN NANOTECNOLOGÍA,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (221,'INGENIERÍA EN NANOTECNOLOGÍA','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="223" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5770,7 +5785,7 @@
       </c>
       <c r="D223" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (222,INGENIERÍA EN NEGOCIOS,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (222,'INGENIERÍA EN NEGOCIOS','GESTION EMPRESARIAL');</v>
       </c>
     </row>
     <row r="224" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5786,7 +5801,7 @@
       </c>
       <c r="D224" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (223,INGENIERÍA EN OBRAS Y SERVICIOS,INGENIERIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (223,'INGENIERÍA EN OBRAS Y SERVICIOS','INGENIERIAS');</v>
       </c>
     </row>
     <row r="225" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5802,7 +5817,7 @@
       </c>
       <c r="D225" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (224,INGENIERÍA EN RECURSOS NATURALES Y AGROPECURIOS,AGRONOMIA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (224,'INGENIERÍA EN RECURSOS NATURALES Y AGROPECURIOS','AGRONOMIA');</v>
       </c>
     </row>
     <row r="226" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5818,7 +5833,7 @@
       </c>
       <c r="D226" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (225,INGENIERÍA EN SISTEMAS,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (225,'INGENIERÍA EN SISTEMAS','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="227" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5834,7 +5849,7 @@
       </c>
       <c r="D227" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (226,INGENIERÍA EN SISTEMAS DE PRODUCCIÓN,INGENIERIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (226,'INGENIERÍA EN SISTEMAS DE PRODUCCIÓN','INGENIERIAS');</v>
       </c>
     </row>
     <row r="228" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5850,7 +5865,7 @@
       </c>
       <c r="D228" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (227,INGENIERÍA EN SISTEMAS PECUARIOS,AGRONOMIA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (227,'INGENIERÍA EN SISTEMAS PECUARIOS','AGRONOMIA');</v>
       </c>
     </row>
     <row r="229" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5866,7 +5881,7 @@
       </c>
       <c r="D229" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (228,INGENIERÍA EN TELEMÁTICA,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (228,'INGENIERÍA EN TELEMÁTICA','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="230" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5882,7 +5897,7 @@
       </c>
       <c r="D230" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (229,INGENIERÍA EN VIDEOJUEGOS,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (229,'INGENIERÍA EN VIDEOJUEGOS','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="231" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5898,7 +5913,7 @@
       </c>
       <c r="D231" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (230,INGENIERIA EN ZOOTECNIA,CIENCIAS VETERINARIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (230,'INGENIERIA EN ZOOTECNIA','CIENCIAS VETERINARIAS');</v>
       </c>
     </row>
     <row r="232" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5914,7 +5929,7 @@
       </c>
       <c r="D232" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (231,INGENIERÍA FORESTAL,INGENIERIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (231,'INGENIERÍA FORESTAL','INGENIERIAS');</v>
       </c>
     </row>
     <row r="233" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5930,7 +5945,7 @@
       </c>
       <c r="D233" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (232,INGENIERÍA GEOGRÁFICA,INGENIERIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (232,'INGENIERÍA GEOGRÁFICA','INGENIERIAS');</v>
       </c>
     </row>
     <row r="234" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5946,7 +5961,7 @@
       </c>
       <c r="D234" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (233,INGENIERÍA INDUSTRIAL,INGENIERIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (233,'INGENIERÍA INDUSTRIAL','INGENIERIAS');</v>
       </c>
     </row>
     <row r="235" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5962,7 +5977,7 @@
       </c>
       <c r="D235" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (234,INGENIERÍA INFORMÁTICA,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (234,'INGENIERÍA INFORMÁTICA','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="236" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5978,7 +5993,7 @@
       </c>
       <c r="D236" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (235,INGENIERÍA INFORMÁTICA EMPRESARIAL,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (235,'INGENIERÍA INFORMÁTICA EMPRESARIAL','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="237" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5994,7 +6009,7 @@
       </c>
       <c r="D237" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (236,INGENIERÍA MECÁNICA,INGENIERIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (236,'INGENIERÍA MECÁNICA','INGENIERIAS');</v>
       </c>
     </row>
     <row r="238" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6010,7 +6025,7 @@
       </c>
       <c r="D238" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (237,INGENIERÍA MECÁNICA ELÉCTRICA,INGENIERIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (237,'INGENIERÍA MECÁNICA ELÉCTRICA','INGENIERIAS');</v>
       </c>
     </row>
     <row r="239" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6026,7 +6041,7 @@
       </c>
       <c r="D239" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (238,INGENIERÍA MECATRÓNICA,INGENIERIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (238,'INGENIERÍA MECATRÓNICA','INGENIERIAS');</v>
       </c>
     </row>
     <row r="240" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6042,7 +6057,7 @@
       </c>
       <c r="D240" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (239,INGENIERÍA QUÍMICA,INGENIERIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (239,'INGENIERÍA QUÍMICA','INGENIERIAS');</v>
       </c>
     </row>
     <row r="241" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6058,7 +6073,7 @@
       </c>
       <c r="D241" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (240,INGENIERÍA SISTEMAS COMPUTACIONALES,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (240,'INGENIERÍA SISTEMAS COMPUTACIONALES','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="242" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6074,7 +6089,7 @@
       </c>
       <c r="D242" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (241,INGENIERÍA TOPOGRÁFICA,INGENIERIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (241,'INGENIERÍA TOPOGRÁFICA','INGENIERIAS');</v>
       </c>
     </row>
     <row r="243" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6090,7 +6105,7 @@
       </c>
       <c r="D243" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (242,INGENIERÍA ZOOTECNIA,CIENCIAS VETERINARIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (242,'INGENIERÍA ZOOTECNIA','CIENCIAS VETERINARIAS');</v>
       </c>
     </row>
     <row r="244" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6106,7 +6121,7 @@
       </c>
       <c r="D244" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (243,INGENIERO AGRÓNOMO,AGRONOMIA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (243,'INGENIERO AGRÓNOMO','AGRONOMIA');</v>
       </c>
     </row>
     <row r="245" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6122,7 +6137,7 @@
       </c>
       <c r="D245" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (244,INHALOTERAPIA,DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (244,'INHALOTERAPIA','DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD');</v>
       </c>
     </row>
     <row r="246" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6138,7 +6153,7 @@
       </c>
       <c r="D246" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (245,INSTALACIONES ELÉCTRICAS,INGENIERIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (245,'INSTALACIONES ELÉCTRICAS','INGENIERIAS');</v>
       </c>
     </row>
     <row r="247" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6154,7 +6169,7 @@
       </c>
       <c r="D247" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (246,INTELIGENCÍA ARTIFICIAL,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (246,'INTELIGENCÍA ARTIFICIAL','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="248" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6170,7 +6185,7 @@
       </c>
       <c r="D248" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (247,INTERVENCIÓN CLÍNICA EN ADOLESCENTES,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (247,'INTERVENCIÓN CLÍNICA EN ADOLESCENTES','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="249" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6186,7 +6201,7 @@
       </c>
       <c r="D249" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (248,INTERVENCIÓN CLÍNICA EN NIÑOS,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (248,'INTERVENCIÓN CLÍNICA EN NIÑOS','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="250" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6202,7 +6217,7 @@
       </c>
       <c r="D250" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (249,INVESTIGACIÓN DE MERCADOS,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (249,'INVESTIGACIÓN DE MERCADOS','GESTION EMPRESARIAL');</v>
       </c>
     </row>
     <row r="251" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6218,7 +6233,7 @@
       </c>
       <c r="D251" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (250,KINESIOLOGÍA,DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (250,'KINESIOLOGÍA','DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD');</v>
       </c>
     </row>
     <row r="252" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6234,7 +6249,7 @@
       </c>
       <c r="D252" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (251,LABORATORISTA,CIENCIAS BASICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (251,'LABORATORISTA','CIENCIAS BASICAS');</v>
       </c>
     </row>
     <row r="253" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6250,7 +6265,7 @@
       </c>
       <c r="D253" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (252,LABORATORISTA CLÍNICO,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (252,'LABORATORISTA CLÍNICO','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="254" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6266,7 +6281,7 @@
       </c>
       <c r="D254" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (253,LENGUA,ESTUDIOS HISTORICOS Y HUMANOS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (253,'LENGUA','ESTUDIOS HISTORICOS Y HUMANOS');</v>
       </c>
     </row>
     <row r="255" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6282,7 +6297,7 @@
       </c>
       <c r="D255" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (254,LETRAS HISPÁNICAS,ESTUDIOS HISTORICOS Y HUMANOS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (254,'LETRAS HISPÁNICAS','ESTUDIOS HISTORICOS Y HUMANOS');</v>
       </c>
     </row>
     <row r="256" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6298,7 +6313,7 @@
       </c>
       <c r="D256" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (255,LITERATURA ALEMANA,ESTUDIOS DE LA CULTURA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (255,'LITERATURA ALEMANA','ESTUDIOS DE LA CULTURA');</v>
       </c>
     </row>
     <row r="257" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6314,7 +6329,7 @@
       </c>
       <c r="D257" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (256,LITERATURA HISPÁNICAS,ESTUDIOS DE LA CULTURA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (256,'LITERATURA HISPÁNICAS','ESTUDIOS DE LA CULTURA');</v>
       </c>
     </row>
     <row r="258" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6330,7 +6345,7 @@
       </c>
       <c r="D258" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>INSERT INTO tb_tematicas VALUES (257,MANEJO DE APARATOS DE ELECTRODIAGNÓSTICO,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (257,'MANEJO DE APARATOS DE ELECTRODIAGNÓSTICO','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="259" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6345,8 +6360,8 @@
         <v>373</v>
       </c>
       <c r="D259" s="1" t="str">
-        <f t="shared" ref="D259:D322" si="10">CONCATENATE("INSERT INTO tb_tematicas VALUES (",A259,",",B259,",",C259,");")</f>
-        <v>INSERT INTO tb_tematicas VALUES (258,MANTENIMIENTO ELÉCTRICO,INGENIERIAS);</v>
+        <f t="shared" ref="D259:D322" si="10">CONCATENATE("INSERT INTO `courseroom`.`tb_tematicas` VALUES (",A259,",'",B259,"','",C259,"');")</f>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (258,'MANTENIMIENTO ELÉCTRICO','INGENIERIAS');</v>
       </c>
     </row>
     <row r="260" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6362,7 +6377,7 @@
       </c>
       <c r="D260" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (259,MANTENIMIENTO INDUSTRIAL,INGENIERIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (259,'MANTENIMIENTO INDUSTRIAL','INGENIERIAS');</v>
       </c>
     </row>
     <row r="261" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6378,7 +6393,7 @@
       </c>
       <c r="D261" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (260,MÁQUINAS DE COMBUSTIÓN INTERNA,INGENIERIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (260,'MÁQUINAS DE COMBUSTIÓN INTERNA','INGENIERIAS');</v>
       </c>
     </row>
     <row r="262" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6394,7 +6409,7 @@
       </c>
       <c r="D262" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (261,MARKETING,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (261,'MARKETING','GESTION EMPRESARIAL');</v>
       </c>
     </row>
     <row r="263" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6410,7 +6425,7 @@
       </c>
       <c r="D263" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (262,MATEMÁTICAS,CIENCIAS BASICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (262,'MATEMÁTICAS','CIENCIAS BASICAS');</v>
       </c>
     </row>
     <row r="264" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6426,7 +6441,7 @@
       </c>
       <c r="D264" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (263,MECÁNICA AUTOMOTRIZ,INGENIERIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (263,'MECÁNICA AUTOMOTRIZ','INGENIERIAS');</v>
       </c>
     </row>
     <row r="265" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6442,7 +6457,7 @@
       </c>
       <c r="D265" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (264,MECÁNICA DIESEL,INGENIERIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (264,'MECÁNICA DIESEL','INGENIERIAS');</v>
       </c>
     </row>
     <row r="266" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6458,7 +6473,7 @@
       </c>
       <c r="D266" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (265,MEDICINA,DISCIPLINAS BASICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (265,'MEDICINA','DISCIPLINAS BASICAS');</v>
       </c>
     </row>
     <row r="267" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6474,7 +6489,7 @@
       </c>
       <c r="D267" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (266,MEDICINA VETERINARIA,CIENCIAS VETERINARIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (266,'MEDICINA VETERINARIA','CIENCIAS VETERINARIAS');</v>
       </c>
     </row>
     <row r="268" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6490,7 +6505,7 @@
       </c>
       <c r="D268" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (267,MÉDICO CIRUJANO,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (267,'MÉDICO CIRUJANO','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="269" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6506,7 +6521,7 @@
       </c>
       <c r="D269" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (268,MÉDICO PARTERO,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (268,'MÉDICO PARTERO','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="270" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6522,7 +6537,7 @@
       </c>
       <c r="D270" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (269,MERCADOTECNIA,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (269,'MERCADOTECNIA','GESTION EMPRESARIAL');</v>
       </c>
     </row>
     <row r="271" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6538,7 +6553,7 @@
       </c>
       <c r="D271" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (270,MERCADOTECNIA INTERNACIONAL,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (270,'MERCADOTECNIA INTERNACIONAL','GESTION EMPRESARIAL');</v>
       </c>
     </row>
     <row r="272" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6554,7 +6569,7 @@
       </c>
       <c r="D272" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (271,MÚSICA,IMAGEN Y SONIDO);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (271,'MÚSICA','IMAGEN Y SONIDO');</v>
       </c>
     </row>
     <row r="273" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6570,7 +6585,7 @@
       </c>
       <c r="D273" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (272,NEGOCIOS INTERNACIONALES,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (272,'NEGOCIOS INTERNACIONALES','GESTION EMPRESARIAL');</v>
       </c>
     </row>
     <row r="274" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6586,7 +6601,7 @@
       </c>
       <c r="D274" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (273,NEONATOLOGÍA,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (273,'NEONATOLOGÍA','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="275" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6602,7 +6617,7 @@
       </c>
       <c r="D275" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (274,NEUMOLOGÍA PEDIÁTRICA,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (274,'NEUMOLOGÍA PEDIÁTRICA','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="276" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6618,7 +6633,7 @@
       </c>
       <c r="D276" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (275,NEUROCIRUGÍA,DISCIPLINAS BASICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (275,'NEUROCIRUGÍA','DISCIPLINAS BASICAS');</v>
       </c>
     </row>
     <row r="277" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6634,7 +6649,7 @@
       </c>
       <c r="D277" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (276,NEUROLINGÜÍSTICA,DISCIPLINAS BASICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (276,'NEUROLINGÜÍSTICA','DISCIPLINAS BASICAS');</v>
       </c>
     </row>
     <row r="278" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6650,7 +6665,7 @@
       </c>
       <c r="D278" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (277,NIVELACIÓN DE LA ENFERMERÍA,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (277,'NIVELACIÓN DE LA ENFERMERÍA','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="279" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6666,7 +6681,7 @@
       </c>
       <c r="D279" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (278,NUTRICIÓN,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (278,'NUTRICIÓN','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="280" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6682,7 +6697,7 @@
       </c>
       <c r="D280" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (279,NUTRICIÓN HUMANA,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (279,'NUTRICIÓN HUMANA','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="281" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6698,7 +6713,7 @@
       </c>
       <c r="D281" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (280,NUTRICIÓN PEDIÁTRICA,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (280,'NUTRICIÓN PEDIÁTRICA','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="282" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6714,7 +6729,7 @@
       </c>
       <c r="D282" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (281,OBSTETRICIA,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (281,'OBSTETRICIA','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="283" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6730,7 +6745,7 @@
       </c>
       <c r="D283" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (282,ODONTOLOGÍA,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (282,'ODONTOLOGÍA','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="284" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6746,7 +6761,7 @@
       </c>
       <c r="D284" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (283,ODONTOPEDIATRIA,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (283,'ODONTOPEDIATRIA','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="285" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6762,7 +6777,7 @@
       </c>
       <c r="D285" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (284,ÓPTICA,DISCIPLINAS BASICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (284,'ÓPTICA','DISCIPLINAS BASICAS');</v>
       </c>
     </row>
     <row r="286" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6778,7 +6793,7 @@
       </c>
       <c r="D286" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (285,OPTOMETRÍA,DISCIPLINAS BASICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (285,'OPTOMETRÍA','DISCIPLINAS BASICAS');</v>
       </c>
     </row>
     <row r="287" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6794,7 +6809,7 @@
       </c>
       <c r="D287" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (286,ORGANIZACIÓN INDUSTRIAL,INGENIERIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (286,'ORGANIZACIÓN INDUSTRIAL','INGENIERIAS');</v>
       </c>
     </row>
     <row r="288" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6810,7 +6825,7 @@
       </c>
       <c r="D288" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (287,ORIENTACIÓN PSICOLÓGICA,DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (287,'ORIENTACIÓN PSICOLÓGICA','DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD');</v>
       </c>
     </row>
     <row r="289" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6826,7 +6841,7 @@
       </c>
       <c r="D289" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (288,OTONEUROLOGÍA,DISCIPLINAS BASICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (288,'OTONEUROLOGÍA','DISCIPLINAS BASICAS');</v>
       </c>
     </row>
     <row r="290" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6842,7 +6857,7 @@
       </c>
       <c r="D290" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (289,OTORRINOLARINGOLOGÍA,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (289,'OTORRINOLARINGOLOGÍA','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="291" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6858,7 +6873,7 @@
       </c>
       <c r="D291" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (290,PEDAGOGÍA,CIENCIAS DE LA EDUCACION);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (290,'PEDAGOGÍA','CIENCIAS DE LA EDUCACION');</v>
       </c>
     </row>
     <row r="292" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6874,7 +6889,7 @@
       </c>
       <c r="D292" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (291,PEDIATRÍA,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (291,'PEDIATRÍA','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="293" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6890,7 +6905,7 @@
       </c>
       <c r="D293" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (292,PERICULTURA,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (292,'PERICULTURA','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="294" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6906,7 +6921,7 @@
       </c>
       <c r="D294" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (293,PERIODISMO,ESTUDIOS DE ESTADO Y SOCIEDAD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (293,'PERIODISMO','ESTUDIOS DE ESTADO Y SOCIEDAD');</v>
       </c>
     </row>
     <row r="295" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6922,7 +6937,7 @@
       </c>
       <c r="D295" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (294,PODOLOGÍA,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (294,'PODOLOGÍA','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="296" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6938,7 +6953,7 @@
       </c>
       <c r="D296" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (295,POLITÉCNICA,CIENCIAS BASICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (295,'POLITÉCNICA','CIENCIAS BASICAS');</v>
       </c>
     </row>
     <row r="297" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6954,7 +6969,7 @@
       </c>
       <c r="D297" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (296,PROGRAMACIÓN DE VIDEOJUEGOS,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (296,'PROGRAMACIÓN DE VIDEOJUEGOS','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="298" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6970,7 +6985,7 @@
       </c>
       <c r="D298" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (297,PROGRAMADOR ANALISTA,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (297,'PROGRAMADOR ANALISTA','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="299" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6986,7 +7001,7 @@
       </c>
       <c r="D299" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (298,PROMOCIÓN DE LA SALUD,DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (298,'PROMOCIÓN DE LA SALUD','DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD');</v>
       </c>
     </row>
     <row r="300" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7002,7 +7017,7 @@
       </c>
       <c r="D300" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (299,PROTESISTA DENTAL,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (299,'PROTESISTA DENTAL','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="301" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7018,7 +7033,7 @@
       </c>
       <c r="D301" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (300,PROTOCOLOS DE COMUNICACIÓN,INGENIERIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (300,'PROTOCOLOS DE COMUNICACIÓN','INGENIERIAS');</v>
       </c>
     </row>
     <row r="302" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7034,7 +7049,7 @@
       </c>
       <c r="D302" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (301,PSICOANALÍSIS,DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (301,'PSICOANALÍSIS','DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD');</v>
       </c>
     </row>
     <row r="303" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7050,7 +7065,7 @@
       </c>
       <c r="D303" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (302,PSICOLOGÍA,DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (302,'PSICOLOGÍA','DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD');</v>
       </c>
     </row>
     <row r="304" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7066,7 +7081,7 @@
       </c>
       <c r="D304" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (303,PSICOLOGÍA DE LA SALUD,DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (303,'PSICOLOGÍA DE LA SALUD','DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD');</v>
       </c>
     </row>
     <row r="305" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7082,7 +7097,7 @@
       </c>
       <c r="D305" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (304,PSICOLOGÍA EDUCATIVA,DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (304,'PSICOLOGÍA EDUCATIVA','DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD');</v>
       </c>
     </row>
     <row r="306" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7098,7 +7113,7 @@
       </c>
       <c r="D306" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (305,PSICOLOGÍA EN TERAPIA FAMILIAR,DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (305,'PSICOLOGÍA EN TERAPIA FAMILIAR','DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD');</v>
       </c>
     </row>
     <row r="307" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7114,7 +7129,7 @@
       </c>
       <c r="D307" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (306,PSICOLOGÍA SOCIAL,DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (306,'PSICOLOGÍA SOCIAL','DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD');</v>
       </c>
     </row>
     <row r="308" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7130,7 +7145,7 @@
       </c>
       <c r="D308" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (307,PSICOONCOLOGIA,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (307,'PSICOONCOLOGIA','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="309" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7146,7 +7161,7 @@
       </c>
       <c r="D309" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (308,PSICOPEDAGOGÍA,DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (308,'PSICOPEDAGOGÍA','DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD');</v>
       </c>
     </row>
     <row r="310" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7162,7 +7177,7 @@
       </c>
       <c r="D310" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (309,PSICOTERAPIA,DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (309,'PSICOTERAPIA','DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD');</v>
       </c>
     </row>
     <row r="311" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7178,7 +7193,7 @@
       </c>
       <c r="D311" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (310,PSICOTERAPIA BREVE SISTÉMICA,DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (310,'PSICOTERAPIA BREVE SISTÉMICA','DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD');</v>
       </c>
     </row>
     <row r="312" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7194,7 +7209,7 @@
       </c>
       <c r="D312" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (311,PSICOTERAPIA INFANTIL,DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (311,'PSICOTERAPIA INFANTIL','DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD');</v>
       </c>
     </row>
     <row r="313" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7210,7 +7225,7 @@
       </c>
       <c r="D313" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (312,PSICOTERAPIA PSICOANALÍTICA,DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (312,'PSICOTERAPIA PSICOANALÍTICA','DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD');</v>
       </c>
     </row>
     <row r="314" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7226,7 +7241,7 @@
       </c>
       <c r="D314" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (313,PUBLICIDAD,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (313,'PUBLICIDAD','GESTION EMPRESARIAL');</v>
       </c>
     </row>
     <row r="315" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7242,7 +7257,7 @@
       </c>
       <c r="D315" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (314,PUERICULTURA,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (314,'PUERICULTURA','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="316" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7258,7 +7273,7 @@
       </c>
       <c r="D316" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (315,QUÍMICA,CIENCIAS BASICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (315,'QUÍMICA','CIENCIAS BASICAS');</v>
       </c>
     </row>
     <row r="317" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7274,7 +7289,7 @@
       </c>
       <c r="D317" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (316,QUÍMICA CLÍNICA,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (316,'QUÍMICA CLÍNICA','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="318" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7290,7 +7305,7 @@
       </c>
       <c r="D318" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (317,QUÍMICA EN ALIMENTOS,CIENCIAS BASICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (317,'QUÍMICA EN ALIMENTOS','CIENCIAS BASICAS');</v>
       </c>
     </row>
     <row r="319" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7306,7 +7321,7 @@
       </c>
       <c r="D319" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (318,QUÍMICA FARMACEÚTICA BIOLÓGICA,CIENCIAS BASICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (318,'QUÍMICA FARMACEÚTICA BIOLÓGICA','CIENCIAS BASICAS');</v>
       </c>
     </row>
     <row r="320" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7322,7 +7337,7 @@
       </c>
       <c r="D320" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (319,QUÍMICA Y FARMACIA,CIENCIAS BASICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (319,'QUÍMICA Y FARMACIA','CIENCIAS BASICAS');</v>
       </c>
     </row>
     <row r="321" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7338,7 +7353,7 @@
       </c>
       <c r="D321" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (320,QUÍMICO BACTERIÓLOGO PARASITÓLOGO,CIENCIAS BASICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (320,'QUÍMICO BACTERIÓLOGO PARASITÓLOGO','CIENCIAS BASICAS');</v>
       </c>
     </row>
     <row r="322" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7354,7 +7369,7 @@
       </c>
       <c r="D322" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>INSERT INTO tb_tematicas VALUES (321,QUÍMICO FARMACEÚTICO BIOLÓGICO,CIENCIAS BASICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (321,'QUÍMICO FARMACEÚTICO BIOLÓGICO','CIENCIAS BASICAS');</v>
       </c>
     </row>
     <row r="323" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7369,8 +7384,8 @@
         <v>362</v>
       </c>
       <c r="D323" s="1" t="str">
-        <f t="shared" ref="D323:D361" si="12">CONCATENATE("INSERT INTO tb_tematicas VALUES (",A323,",",B323,",",C323,");")</f>
-        <v>INSERT INTO tb_tematicas VALUES (322,QUÍMICO FARMACÉUTICO INDUSTRIAL,CIENCIAS BASICAS);</v>
+        <f t="shared" ref="D323:D361" si="12">CONCATENATE("INSERT INTO `courseroom`.`tb_tematicas` VALUES (",A323,",'",B323,"','",C323,"');")</f>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (322,'QUÍMICO FARMACÉUTICO INDUSTRIAL','CIENCIAS BASICAS');</v>
       </c>
     </row>
     <row r="324" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7386,7 +7401,7 @@
       </c>
       <c r="D324" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>INSERT INTO tb_tematicas VALUES (323,QUÍMICO FARMACOBIÓLOGO,CIENCIAS BASICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (323,'QUÍMICO FARMACOBIÓLOGO','CIENCIAS BASICAS');</v>
       </c>
     </row>
     <row r="325" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7402,7 +7417,7 @@
       </c>
       <c r="D325" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>INSERT INTO tb_tematicas VALUES (324,QUÍMICO INDUSTRIAL,CIENCIAS BASICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (324,'QUÍMICO INDUSTRIAL','CIENCIAS BASICAS');</v>
       </c>
     </row>
     <row r="326" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7418,7 +7433,7 @@
       </c>
       <c r="D326" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>INSERT INTO tb_tematicas VALUES (325,QUIROPRÁCTICA,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (325,'QUIROPRÁCTICA','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="327" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7434,7 +7449,7 @@
       </c>
       <c r="D327" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>INSERT INTO tb_tematicas VALUES (326,RADIOLOGÍA,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (326,'RADIOLOGÍA','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="328" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7450,7 +7465,7 @@
       </c>
       <c r="D328" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>INSERT INTO tb_tematicas VALUES (327,RADIOLOGÍA E IMAGEN,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (327,'RADIOLOGÍA E IMAGEN','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="329" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7466,7 +7481,7 @@
       </c>
       <c r="D329" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>INSERT INTO tb_tematicas VALUES (328,RECURSOS HUMANOS,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (328,'RECURSOS HUMANOS','GESTION EMPRESARIAL');</v>
       </c>
     </row>
     <row r="330" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7482,7 +7497,7 @@
       </c>
       <c r="D330" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>INSERT INTO tb_tematicas VALUES (329,REDES DE COMUNICACIÓN,INGENIERIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (329,'REDES DE COMUNICACIÓN','INGENIERIAS');</v>
       </c>
     </row>
     <row r="331" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7498,7 +7513,7 @@
       </c>
       <c r="D331" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>INSERT INTO tb_tematicas VALUES (330,REHABILITACIÓN INTEGRAL,DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (330,'REHABILITACIÓN INTEGRAL','DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD');</v>
       </c>
     </row>
     <row r="332" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7514,7 +7529,7 @@
       </c>
       <c r="D332" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>INSERT INTO tb_tematicas VALUES (331,RELACIONES COMERCIALES,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (331,'RELACIONES COMERCIALES','GESTION EMPRESARIAL');</v>
       </c>
     </row>
     <row r="333" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7530,7 +7545,7 @@
       </c>
       <c r="D333" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>INSERT INTO tb_tematicas VALUES (332,RELACIONES INTERNACIONALES,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (332,'RELACIONES INTERNACIONALES','GESTION EMPRESARIAL');</v>
       </c>
     </row>
     <row r="334" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7546,7 +7561,7 @@
       </c>
       <c r="D334" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>INSERT INTO tb_tematicas VALUES (333,REUMATOLOGÍA PEDIÁTRICA,DISCIPLINAS BASICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (333,'REUMATOLOGÍA PEDIÁTRICA','DISCIPLINAS BASICAS');</v>
       </c>
     </row>
     <row r="335" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7562,7 +7577,7 @@
       </c>
       <c r="D335" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>INSERT INTO tb_tematicas VALUES (334,ROBÓTICA,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (334,'ROBÓTICA','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="336" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7578,7 +7593,7 @@
       </c>
       <c r="D336" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>INSERT INTO tb_tematicas VALUES (335,SALUD PÚBLICA,DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (335,'SALUD PÚBLICA','DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD');</v>
       </c>
     </row>
     <row r="337" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7594,7 +7609,7 @@
       </c>
       <c r="D337" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>INSERT INTO tb_tematicas VALUES (336,SECRETARIA EJECUTIVA BILINGÜE,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (336,'SECRETARIA EJECUTIVA BILINGÜE','GESTION EMPRESARIAL');</v>
       </c>
     </row>
     <row r="338" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7610,7 +7625,7 @@
       </c>
       <c r="D338" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>INSERT INTO tb_tematicas VALUES (337,SECRETARIADO,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (337,'SECRETARIADO','GESTION EMPRESARIAL');</v>
       </c>
     </row>
     <row r="339" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7626,7 +7641,7 @@
       </c>
       <c r="D339" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>INSERT INTO tb_tematicas VALUES (338,SECRETARIADO BILINGÜE,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (338,'SECRETARIADO BILINGÜE','GESTION EMPRESARIAL');</v>
       </c>
     </row>
     <row r="340" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7642,7 +7657,7 @@
       </c>
       <c r="D340" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>INSERT INTO tb_tematicas VALUES (339,SECRETARIADO EN COMPUTACIÓN,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (339,'SECRETARIADO EN COMPUTACIÓN','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="341" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7658,7 +7673,7 @@
       </c>
       <c r="D341" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>INSERT INTO tb_tematicas VALUES (340,SISTEMA EDUCATIVO NACIONAL,CIENCIAS DE LA EDUCACION);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (340,'SISTEMA EDUCATIVO NACIONAL','CIENCIAS DE LA EDUCACION');</v>
       </c>
     </row>
     <row r="342" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7674,7 +7689,7 @@
       </c>
       <c r="D342" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>INSERT INTO tb_tematicas VALUES (341,SISTEMA EN COMPUTACIÓN ADMINISTRATIVA,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (341,'SISTEMA EN COMPUTACIÓN ADMINISTRATIVA','GESTION EMPRESARIAL');</v>
       </c>
     </row>
     <row r="343" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7690,7 +7705,7 @@
       </c>
       <c r="D343" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>INSERT INTO tb_tematicas VALUES (342,SISTEMAS DE INFORMACIÓN,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (342,'SISTEMAS DE INFORMACIÓN','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="344" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7706,7 +7721,7 @@
       </c>
       <c r="D344" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>INSERT INTO tb_tematicas VALUES (343,SISTEMAS INFORMÁTICOS,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (343,'SISTEMAS INFORMÁTICOS','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="345" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7722,7 +7737,7 @@
       </c>
       <c r="D345" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>INSERT INTO tb_tematicas VALUES (344,SOCIOLOGÍA,ESTUDIOS POLITICOS Y SOCIALES);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (344,'SOCIOLOGÍA','ESTUDIOS POLITICOS Y SOCIALES');</v>
       </c>
     </row>
     <row r="346" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7738,7 +7753,7 @@
       </c>
       <c r="D346" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>INSERT INTO tb_tematicas VALUES (345,TÉCNICO RADIÓLOGO,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (345,'TÉCNICO RADIÓLOGO','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="347" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7754,7 +7769,7 @@
       </c>
       <c r="D347" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>INSERT INTO tb_tematicas VALUES (346,TECNOLOGÍA INFORMÁTICA,TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (346,'TECNOLOGÍA INFORMÁTICA','TECNOLOGIAS PARA LA INTEGRACION CIBER-HUMANA');</v>
       </c>
     </row>
     <row r="348" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7770,7 +7785,7 @@
       </c>
       <c r="D348" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>INSERT INTO tb_tematicas VALUES (347,TERAPIA DE LENGUAJE,DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (347,'TERAPIA DE LENGUAJE','DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD');</v>
       </c>
     </row>
     <row r="349" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7786,7 +7801,7 @@
       </c>
       <c r="D349" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>INSERT INTO tb_tematicas VALUES (348,TERAPIA FAMILIAR,DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (348,'TERAPIA FAMILIAR','DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD');</v>
       </c>
     </row>
     <row r="350" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7802,7 +7817,7 @@
       </c>
       <c r="D350" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>INSERT INTO tb_tematicas VALUES (349,TERAPIA FÍSICA,DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (349,'TERAPIA FÍSICA','DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD');</v>
       </c>
     </row>
     <row r="351" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7818,7 +7833,7 @@
       </c>
       <c r="D351" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>INSERT INTO tb_tematicas VALUES (350,TERAPIA OCUPACIONAL,DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (350,'TERAPIA OCUPACIONAL','DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD');</v>
       </c>
     </row>
     <row r="352" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7834,7 +7849,7 @@
       </c>
       <c r="D352" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>INSERT INTO tb_tematicas VALUES (351,TERAPIA RESPIRATORIA,DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (351,'TERAPIA RESPIRATORIA','DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD');</v>
       </c>
     </row>
     <row r="353" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7850,7 +7865,7 @@
       </c>
       <c r="D353" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>INSERT INTO tb_tematicas VALUES (352,TERAPISTA EN COMUNICACIÓN HUMANA,DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (352,'TERAPISTA EN COMUNICACIÓN HUMANA','DISCIPLINAS PARA EL DESARROLLO, PROMOCION Y PRESERVACION DE LA SALUD');</v>
       </c>
     </row>
     <row r="354" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7866,7 +7881,7 @@
       </c>
       <c r="D354" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>INSERT INTO tb_tematicas VALUES (353,TRABAJO SOCIAL,ESTUDIOS POLITICOS Y SOCIALES);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (353,'TRABAJO SOCIAL','ESTUDIOS POLITICOS Y SOCIALES');</v>
       </c>
     </row>
     <row r="355" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7882,7 +7897,7 @@
       </c>
       <c r="D355" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>INSERT INTO tb_tematicas VALUES (354,TURISMO,GESTION EMPRESARIAL);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (354,'TURISMO','GESTION EMPRESARIAL');</v>
       </c>
     </row>
     <row r="356" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7898,7 +7913,7 @@
       </c>
       <c r="D356" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>INSERT INTO tb_tematicas VALUES (355,URBANISMO,IMAGEN Y SONIDO);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (355,'URBANISMO','IMAGEN Y SONIDO');</v>
       </c>
     </row>
     <row r="357" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7914,7 +7929,7 @@
       </c>
       <c r="D357" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>INSERT INTO tb_tematicas VALUES (356,URBANÍSTICA Y MEDIO AMBIENTE,IMAGEN Y SONIDO);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (356,'URBANÍSTICA Y MEDIO AMBIENTE','IMAGEN Y SONIDO');</v>
       </c>
     </row>
     <row r="358" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7930,7 +7945,7 @@
       </c>
       <c r="D358" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>INSERT INTO tb_tematicas VALUES (357,URGENCIAS MÉDICAS BÁSICO,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (357,'URGENCIAS MÉDICAS BÁSICO','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="359" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7946,7 +7961,7 @@
       </c>
       <c r="D359" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>INSERT INTO tb_tematicas VALUES (358,UROLOGÍA GINECOLÓGICA,DISCIPLINAS CLINICAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (358,'UROLOGÍA GINECOLÓGICA','DISCIPLINAS CLINICAS');</v>
       </c>
     </row>
     <row r="360" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7962,7 +7977,7 @@
       </c>
       <c r="D360" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>INSERT INTO tb_tematicas VALUES (359,VETERINARIA,CIENCIAS VETERINARIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (359,'VETERINARIA','CIENCIAS VETERINARIAS');</v>
       </c>
     </row>
     <row r="361" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7978,7 +7993,7 @@
       </c>
       <c r="D361" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>INSERT INTO tb_tematicas VALUES (360,ZOOTECNIA,CIENCIAS VETERINARIAS);</v>
+        <v>INSERT INTO `courseroom`.`tb_tematicas` VALUES (360,'ZOOTECNIA','CIENCIAS VETERINARIAS');</v>
       </c>
     </row>
   </sheetData>

</xml_diff>